<commit_message>
feat: web funcionalidade de baixar achados dos cruzamentos em funcionamento
</commit_message>
<xml_diff>
--- a/web/uploads/servidores_cruzamento.xlsx
+++ b/web/uploads/servidores_cruzamento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="7">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -247,10 +247,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,6 +431,414 @@
         <v>999999999.99</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>20412634524</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>10641944494</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>11791847506</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>16785564396</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>16862797558</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>10224458768</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>21447448571</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>16553730149</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>11742077000</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>12017882684</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>16863150477</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>16430525776</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>12798121452</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>16398233752</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>12580267486</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>16146164616</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>20453212950</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>16361202381</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>20767551642</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>13378191421</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>16400283375</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>12493595779</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>12944297653</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>99999999999</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>16140231826</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>999999999.99</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>